<commit_message>
feature: now the scripts runs in hidden mode
</commit_message>
<xml_diff>
--- a/documents/Activities.xlsx
+++ b/documents/Activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dracc\OneDrive\Documentos\Globpar\Proyectos\excel\excel-convertion-manual-parsing\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCCAED9-0B9E-429C-AC0B-7628920FFD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1FB7B3-39FE-4248-A6A4-69C27EFE5A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1229434-66A6-2944-AAAC-42BDEDF68F5A}"/>
+    <workbookView xWindow="2355" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{D1229434-66A6-2944-AAAC-42BDEDF68F5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Doc4" sheetId="2" r:id="rId1"/>
@@ -12588,6 +12588,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC43274AD24C8A4CB58F6E2616454155" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab09bab7d31d2d506f1fa9cd473ea066">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5251f7ab-246d-47af-a628-62d5055d0c18" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6fe188b6358f467fd736c66e8750084" ns2:_="">
     <xsd:import namespace="5251f7ab-246d-47af-a628-62d5055d0c18"/>
@@ -12737,15 +12746,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F795DEA1-15DB-450F-BEB4-AD2D64D6DEF8}">
   <ds:schemaRefs>
@@ -12763,6 +12763,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DDAFEC1-5412-4857-BAE8-02C39C58CFFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E46302E3-F08A-4F75-8171-D677B09598FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12778,12 +12786,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DDAFEC1-5412-4857-BAE8-02C39C58CFFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>